<commit_message>
Update Charges section header in taxbuddy template
</commit_message>
<xml_diff>
--- a/src/assets/files/TaxBuddy Cg Template.xlsx
+++ b/src/assets/files/TaxBuddy Cg Template.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="80">
   <si>
     <t>Important Points to be considered before you proceed ahead.</t>
   </si>
@@ -345,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -392,6 +392,9 @@
     <xf borderId="1" fillId="2" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
@@ -2412,7 +2415,9 @@
       <c r="A25" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="11"/>
+      <c r="B25" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
@@ -10758,7 +10763,9 @@
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="11"/>
+      <c r="B22" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -17966,7 +17973,9 @@
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="11"/>
+      <c r="B22" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -25311,7 +25320,9 @@
       <c r="A24" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="4"/>
+      <c r="B24" s="23" t="s">
+        <v>14</v>
+      </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -25391,7 +25402,7 @@
       <c r="A27" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="23"/>
+      <c r="B27" s="24"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -31895,7 +31906,9 @@
       <c r="A24" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="4"/>
+      <c r="B24" s="23" t="s">
+        <v>14</v>
+      </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -31983,7 +31996,7 @@
       <c r="A27" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="23"/>
+      <c r="B27" s="24"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -39315,7 +39328,9 @@
       <c r="A24" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="4"/>
+      <c r="B24" s="23" t="s">
+        <v>14</v>
+      </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -39403,7 +39418,7 @@
       <c r="A27" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="23"/>
+      <c r="B27" s="24"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -46230,7 +46245,7 @@
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="24"/>
+      <c r="C5" s="25"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
       <c r="F5" s="4"/>
@@ -46257,7 +46272,7 @@
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
-      <c r="C6" s="24"/>
+      <c r="C6" s="25"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="4"/>
@@ -46284,7 +46299,7 @@
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
-      <c r="C7" s="24"/>
+      <c r="C7" s="25"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="4"/>
@@ -46311,7 +46326,7 @@
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
-      <c r="C8" s="24"/>
+      <c r="C8" s="25"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="4"/>

</xml_diff>